<commit_message>
commit modifications v1 made, need to install packages and solvers
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>6514.999999999998</v>
+        <v>5695</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>6518</v>
+        <v>5697.999999999956</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>6521.999659525188</v>
+        <v>5702</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>6525</v>
+        <v>5705</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>6519.999999999996</v>
+        <v>5700</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>6511</v>
+        <v>5691</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>6520.999999999694</v>
+        <v>5700.999999999956</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>6526</v>
+        <v>5705.999999999985</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit test run need implement further modifications
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>5695</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>5697.999999999956</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>5702</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>5705</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>5700</v>
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>5691</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>5700.999999999956</v>
+        <v>203.3999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>5705.999999999985</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit `infeasible` objective problem to be fixed. Partial output
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>181</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>200</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>200</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>189</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>177</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>203.3999999999996</v>
+        <v>152.3999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>200</v>
+        <v>185.2000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit model running, need to debug and discuss
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>138</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>190</v>
+        <v>176.6000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>152.3999999999996</v>
+        <v>162.3999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>185.2000000000007</v>
+        <v>195.2000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit functional model need to compare with doc
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>176.6000000000004</v>
+        <v>175.6000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>162.3999999999996</v>
+        <v>161.3999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>195.2000000000007</v>
+        <v>194.2000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit need to complete debugging, need to confirm indices for alpha and l
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -348,42 +348,42 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1">
-        <v>161</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>147</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>135</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>175.6000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>161.3999999999996</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>194.2000000000007</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit lowest objective value obtained so far
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -353,36 +353,46 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>0</v>
+        <v>120.2000000000006</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>0</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>0</v>
+        <v>191.1999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>0</v>
+        <v>189.1999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>0</v>
+        <v>148.2000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>0</v>
+        <v>182.2000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
commit all constraints feasible model
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -353,42 +353,42 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>120.2000000000006</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>110</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>191.1999999999998</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>189.1999999999998</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>148.2000000000006</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>182.2000000000005</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>109</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>200</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:1">

</xml_diff>

<commit_message>
commit model 3 output for analysis
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -353,42 +353,42 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>114</v>
+        <v>263.6000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>140.6000000000004</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>142.2000000000007</v>
+        <v>203.2000000000007</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>190</v>
+        <v>233.2000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>210</v>
+        <v>218.8000000000011</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>130.2000000000007</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:1">

</xml_diff>

<commit_message>
commit corrected model output
</commit_message>
<xml_diff>
--- a/assets/generated/model3/ArrivalAtCustomerTime.xlsx
+++ b/assets/generated/model3/ArrivalAtCustomerTime.xlsx
@@ -353,42 +353,42 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2">
-        <v>194</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3">
-        <v>263.6000000000004</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4">
-        <v>201</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5">
-        <v>203.2000000000007</v>
+        <v>238.3999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6">
-        <v>190</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7">
-        <v>233.2000000000007</v>
+        <v>268.5999999999985</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8">
-        <v>218.8000000000011</v>
+        <v>254.1999999999989</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9">
-        <v>211</v>
+        <v>293.3999999999996</v>
       </c>
     </row>
     <row r="10" spans="1:1">

</xml_diff>